<commit_message>
corrected father name issue
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ankit\LMI\ReportsAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF39BC82-7F43-459D-8F94-CB9806D04B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96CA882-D5F7-4B06-B728-5D63116328E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>The effects of your behavior may not be apparent to you, but your scores indicate that they need urgent attention. Sometimes we learn to behave in a certain way because it makes us feel good, but not everything that feels good is healthy in the long run. Observe what you are doing or avoiding daily. Learn to differentiate between what actions are helpful and unhelpful in the long run. Think of the consequences of your actions for yourself and others in both the short and long term. For example, avoiding studies feels good but isn’t helpful in the long run. Practice behavioral habits that will be beneficial for you and others. Also, practice avoiding actions that are unhelpful or harmful. Even if some of your actions seem beyond control, they can be managed. Seek assistance to learn behavioral management techniques.</t>
   </si>
   <si>
-    <t>Thinking</t>
-  </si>
-  <si>
     <t>Good thoughts will turn into good actions! You are doing a great job in positively dealing with your thoughts. Continue to manage your thoughts well.</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>Your scores suggest that you are experiencing negative thoughts that can be distressing, and these thoughts are in a concerning range. Our brain is a constant thinking machine. When something happens that we don’t like, we can have negative thoughts. Do not believe all negative thoughts. If your thoughts continue to be troublesome, seek assistance from your parents or any trusted adults and talk to a therapist.</t>
   </si>
   <si>
-    <t>Body_signals</t>
-  </si>
-  <si>
     <t>Your body seems to be happy with how you are taking care of it! Kudos to you for listening to your body! Continue to manage your body’s health.</t>
   </si>
   <si>
@@ -154,9 +148,6 @@
     <t>Your physical health needs urgent attention. There are many causes of bodily signals, and most of them are normal. Sometimes you feel uncomfortable in your body, and that can be a signal for the body to take action. For example, hunger signals you to eat food, thirst signals you to drink water, and pain signals you to take action or rest. Prolonged and intense distress needs to be evaluated by a doctor. Get your regular health check-up done if you haven't had one in the last six months. If you are already aware of your physical condition and taking medical assistance, stay on track with the doctor’s advice.</t>
   </si>
   <si>
-    <t>Emotions</t>
-  </si>
-  <si>
     <t>Congrats on how well you are managing your emotions! Continue the good work.</t>
   </si>
   <si>
@@ -181,7 +172,16 @@
     <t>The overall scores are problematic. The details provided below should be checked for the issues being faced. These issues require additional evaluation and assistance. A consultation with a counselor or psychologist is advised. Many people go through this during adolescence and are able to successfully deal with the challenges they are going through. This is the right time to take action. Waiting for problems to resolve on their own without taking action can make them worse. Take a look at each section so you can take action today.</t>
   </si>
   <si>
-    <t>Composite scores</t>
+    <t>thinking</t>
+  </si>
+  <si>
+    <t>body_signals</t>
+  </si>
+  <si>
+    <t>emotions</t>
+  </si>
+  <si>
+    <t>composite_score</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A39" sqref="A39:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -804,7 +804,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -813,12 +813,12 @@
         <v>5</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B27" s="1">
         <v>6</v>
@@ -827,12 +827,12 @@
         <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B28" s="1">
         <v>11</v>
@@ -841,12 +841,12 @@
         <v>15</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B29" s="1">
         <v>16</v>
@@ -855,12 +855,12 @@
         <v>20</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -869,12 +869,12 @@
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B31" s="1">
         <v>4</v>
@@ -883,12 +883,12 @@
         <v>6</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B32" s="1">
         <v>7</v>
@@ -897,12 +897,12 @@
         <v>9</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B33" s="1">
         <v>10</v>
@@ -911,12 +911,12 @@
         <v>12</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
@@ -925,12 +925,12 @@
         <v>7</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B35" s="1">
         <v>8</v>
@@ -939,12 +939,12 @@
         <v>14</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B36" s="1">
         <v>15</v>
@@ -953,12 +953,12 @@
         <v>21</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B37" s="1">
         <v>22</v>
@@ -967,7 +967,7 @@
         <v>28</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -981,7 +981,7 @@
         <v>32</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -995,7 +995,7 @@
         <v>64</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
         <v>96</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,7 +1023,7 @@
         <v>128</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed composite score last limit
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ankit\LMI\ReportsAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96CA882-D5F7-4B06-B728-5D63116328E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CA815D-B423-4C98-9C4D-B4FC3DCC7CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,8 +446,8 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:A41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1020,7 @@
         <v>97</v>
       </c>
       <c r="C41" s="1">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
added hindi report support
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ankit\LMI\ReportsAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CA815D-B423-4C98-9C4D-B4FC3DCC7CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E992F099-14BA-439E-8F4A-C4A3B31C25ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$41</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -446,7 +449,7 @@
   </sheetPr>
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -530,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
@@ -541,10 +544,10 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -555,10 +558,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
@@ -569,10 +572,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>13</v>
@@ -586,7 +589,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>15</v>
@@ -597,10 +600,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
         <v>4</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
@@ -611,10 +614,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>17</v>
@@ -625,10 +628,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>18</v>
@@ -642,7 +645,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>20</v>
@@ -653,10 +656,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>21</v>
@@ -667,10 +670,10 @@
         <v>19</v>
       </c>
       <c r="B16" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>22</v>
@@ -681,10 +684,10 @@
         <v>19</v>
       </c>
       <c r="B17" s="1">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>23</v>
@@ -754,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>30</v>
@@ -765,10 +768,10 @@
         <v>29</v>
       </c>
       <c r="B23" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>31</v>
@@ -779,10 +782,10 @@
         <v>29</v>
       </c>
       <c r="B24" s="1">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C24" s="1">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>32</v>
@@ -793,10 +796,10 @@
         <v>29</v>
       </c>
       <c r="B25" s="1">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C25" s="1">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>33</v>
@@ -922,7 +925,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>42</v>
@@ -933,10 +936,10 @@
         <v>52</v>
       </c>
       <c r="B35" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C35" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>43</v>
@@ -947,10 +950,10 @@
         <v>52</v>
       </c>
       <c r="B36" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C36" s="1">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>44</v>
@@ -961,10 +964,10 @@
         <v>52</v>
       </c>
       <c r="B37" s="1">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C37" s="1">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>45</v>
@@ -978,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="1">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>46</v>
@@ -989,10 +992,10 @@
         <v>53</v>
       </c>
       <c r="B39" s="1">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C39" s="1">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>47</v>
@@ -1003,10 +1006,10 @@
         <v>53</v>
       </c>
       <c r="B40" s="1">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C40" s="1">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>48</v>
@@ -1017,16 +1020,17 @@
         <v>53</v>
       </c>
       <c r="B41" s="1">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C41" s="1">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D41" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>